<commit_message>
tweak park can counter
</commit_message>
<xml_diff>
--- a/Can Logs Gen1 Knob/Gen 1 Knob Logs/Gen1 Jag Gearknob Findings.xlsx
+++ b/Can Logs Gen1 Knob/Gen 1 Knob Logs/Gen1 Jag Gearknob Findings.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomde\Documents\Electric Drives\OEM\JAguar\Control Knob Jag\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomde\Documents\GitHub\Land-Rover-Gearknob\Can Logs Gen1 Knob\Gen 1 Knob Logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D0F1425-A190-4369-A8F2-A247503A8EE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7C88421-DF31-49E9-AA47-B724CA379921}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="-10760" windowWidth="19200" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7992" yWindow="0" windowWidth="15048" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -577,8 +577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1005,14 +1005,14 @@
         <v>51</v>
       </c>
       <c r="F44">
-        <f t="shared" ref="F44:F47" si="4">HEX2DEC(E44)</f>
+        <f>HEX2DEC(E44)</f>
         <v>14</v>
       </c>
       <c r="G44" s="5">
         <v>90</v>
       </c>
       <c r="H44">
-        <f t="shared" ref="H44:H47" si="5">HEX2DEC(G44)</f>
+        <f t="shared" ref="H44:H47" si="4">HEX2DEC(G44)</f>
         <v>144</v>
       </c>
       <c r="I44">
@@ -1035,14 +1035,14 @@
         <v>51</v>
       </c>
       <c r="F45">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="F44:F47" si="5">HEX2DEC(E45)</f>
         <v>14</v>
       </c>
       <c r="G45" s="5">
         <v>11</v>
       </c>
       <c r="H45">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>17</v>
       </c>
       <c r="I45">
@@ -1065,14 +1065,14 @@
         <v>51</v>
       </c>
       <c r="F46">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>14</v>
       </c>
       <c r="G46" s="5">
         <v>12</v>
       </c>
       <c r="H46">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
       <c r="I46">
@@ -1095,14 +1095,14 @@
         <v>51</v>
       </c>
       <c r="F47">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>14</v>
       </c>
       <c r="G47" s="5">
         <v>14</v>
       </c>
       <c r="H47">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
       <c r="I47">

</xml_diff>